<commit_message>
add QLFeatures_table as of today implementation status
</commit_message>
<xml_diff>
--- a/docs/QLFeatures_Table_Template.xlsx
+++ b/docs/QLFeatures_Table_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judith Michael\Documents\Publikationen\_SVNpaper\trunk\xx.LanguageWorkbenchComparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\git\github\gemoc\ql-gemoc-lwb2025\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D74C18-DB67-41E3-A593-1FC6C0DEF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA392CC1-504E-4774-926E-F4FDF867305E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2160" windowWidth="16845" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Syntax</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>Please add a comment in this case what partially means</t>
+  </si>
+  <si>
+    <t>Cycles are detected at runtime, they takes into account the current visibilty of the referred Questions which cannot be statically validated</t>
+  </si>
+  <si>
+    <t>in both graphical and textual editors</t>
+  </si>
+  <si>
+    <t>a simple dump in xmi was done, even if it contains all informations entered by the user, a more dedicated save format would have been nicer</t>
+  </si>
+  <si>
+    <t>Actually, in the implementation, the question definition and question application condition are separated,  this case is not relevant as it doesn't matter which condition activated the rendering of the question</t>
+  </si>
+  <si>
+    <t>Verified at runtime only, static validation not implemented</t>
   </si>
 </sst>
 </file>
@@ -244,10 +259,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -258,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -539,7 +553,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,13 +566,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -566,50 +580,60 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="E3" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="E5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
     </row>
@@ -617,116 +641,156 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="E7" s="9" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="E7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="B11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="C22" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add static typechecking to the challenge docs
</commit_message>
<xml_diff>
--- a/docs/QLFeatures_Table_Template.xlsx
+++ b/docs/QLFeatures_Table_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\git\github\gemoc\ql-gemoc-lwb2025\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA392CC1-504E-4774-926E-F4FDF867305E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D3EC69-0318-472E-AC3F-3A7A8F10068A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2160" windowWidth="16845" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Please add a comment in this case what partially means</t>
   </si>
   <si>
-    <t>Cycles are detected at runtime, they takes into account the current visibilty of the referred Questions which cannot be statically validated</t>
-  </si>
-  <si>
     <t>in both graphical and textual editors</t>
   </si>
   <si>
@@ -126,7 +123,10 @@
     <t>Actually, in the implementation, the question definition and question application condition are separated,  this case is not relevant as it doesn't matter which condition activated the rendering of the question</t>
   </si>
   <si>
-    <t>Verified at runtime only, static validation not implemented</t>
+    <t>static validation and runtime validation implemented</t>
+  </si>
+  <si>
+    <t>Cycles are detected at runtime, they takes into account the current visibilty of the referred Questions which cannot be statically validated since they depends on runtime values</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +628,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>24</v>
@@ -662,10 +662,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>